<commit_message>
Added Missing Column (AmountRaised) in Campaigns table and Data init
</commit_message>
<xml_diff>
--- a/Dataset/Final_Dataset.xlsx
+++ b/Dataset/Final_Dataset.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bisha\OneDrive\Desktop\Modern Database\Final Assesment\Dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92076311-B71A-47C3-B9B2-564BA24BDC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Volunteers" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
     <sheet name="Campaign_Resource" sheetId="8" r:id="rId8"/>
     <sheet name="Impact_Resource" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -912,11 +918,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -980,13 +986,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1024,7 +1038,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1058,6 +1072,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1092,9 +1107,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1267,14 +1283,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1314,7 +1330,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1334,7 +1350,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1354,7 +1370,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1374,7 +1390,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1394,7 +1410,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1414,7 +1430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1434,7 +1450,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1454,7 +1470,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1474,7 +1490,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1494,7 +1510,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1514,7 +1530,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1534,7 +1550,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1554,7 +1570,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1574,7 +1590,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1594,7 +1610,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1614,7 +1630,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1634,7 +1650,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1654,7 +1670,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1674,7 +1690,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1694,7 +1710,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1714,7 +1730,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1734,7 +1750,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1754,7 +1770,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1774,7 +1790,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1794,7 +1810,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1814,7 +1830,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1834,7 +1850,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1854,7 +1870,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1874,7 +1890,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1894,7 +1910,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1914,7 +1930,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1934,7 +1950,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1954,7 +1970,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1974,7 +1990,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1994,7 +2010,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2014,7 +2030,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2034,7 +2050,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2054,7 +2070,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2074,7 +2090,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2100,14 +2116,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>125</v>
       </c>
@@ -2127,7 +2152,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2147,7 +2172,7 @@
         <v>103033</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2167,7 +2192,7 @@
         <v>99426</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2187,7 +2212,7 @@
         <v>87196</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2207,7 +2232,7 @@
         <v>118830</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2227,7 +2252,7 @@
         <v>60284</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2247,7 +2272,7 @@
         <v>151668</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2267,7 +2292,7 @@
         <v>165491</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2287,7 +2312,7 @@
         <v>140698</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2307,7 +2332,7 @@
         <v>112457</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2327,7 +2352,7 @@
         <v>168912</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2347,7 +2372,7 @@
         <v>150592</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2367,7 +2392,7 @@
         <v>166532</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2387,7 +2412,7 @@
         <v>106041</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2407,7 +2432,7 @@
         <v>69786</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2427,7 +2452,7 @@
         <v>153841</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2447,7 +2472,7 @@
         <v>123369</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2467,7 +2492,7 @@
         <v>146308</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2487,7 +2512,7 @@
         <v>153935</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2507,7 +2532,7 @@
         <v>98524</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2533,14 +2558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>156</v>
       </c>
@@ -2560,7 +2585,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2580,7 +2605,7 @@
         <v>45380</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2600,7 +2625,7 @@
         <v>45402</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2620,7 +2645,7 @@
         <v>45533</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2640,7 +2665,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2660,7 +2685,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2680,7 +2705,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2700,7 +2725,7 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2720,7 +2745,7 @@
         <v>45428</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2740,7 +2765,7 @@
         <v>45356</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2760,7 +2785,7 @@
         <v>45362</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2780,7 +2805,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2800,7 +2825,7 @@
         <v>45414</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2820,7 +2845,7 @@
         <v>45497</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2840,7 +2865,7 @@
         <v>45549</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2860,7 +2885,7 @@
         <v>45516</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2880,7 +2905,7 @@
         <v>45467</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2900,7 +2925,7 @@
         <v>45458</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2920,7 +2945,7 @@
         <v>45548</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2940,7 +2965,7 @@
         <v>45518</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2960,7 +2985,7 @@
         <v>45369</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2980,7 +3005,7 @@
         <v>45345</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3000,7 +3025,7 @@
         <v>45449</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3020,7 +3045,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3040,7 +3065,7 @@
         <v>45349</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3060,7 +3085,7 @@
         <v>45318</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3080,7 +3105,7 @@
         <v>45316</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3100,7 +3125,7 @@
         <v>45300</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3120,7 +3145,7 @@
         <v>45383</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3140,7 +3165,7 @@
         <v>45491</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3166,14 +3191,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>243</v>
       </c>
@@ -3187,7 +3212,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3201,7 +3226,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3215,7 +3240,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3229,7 +3254,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3243,7 +3268,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3257,7 +3282,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3271,7 +3296,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3285,7 +3310,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3299,7 +3324,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3313,7 +3338,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3327,7 +3352,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3341,7 +3366,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3355,7 +3380,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3369,7 +3394,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3383,7 +3408,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3403,14 +3428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>273</v>
       </c>
@@ -3424,7 +3449,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3438,7 +3463,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3452,7 +3477,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3466,7 +3491,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3480,7 +3505,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3494,7 +3519,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3508,7 +3533,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3522,7 +3547,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3536,7 +3561,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3550,7 +3575,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3570,14 +3595,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3585,7 +3610,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>35</v>
       </c>
@@ -3593,7 +3618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>34</v>
       </c>
@@ -3601,7 +3626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16</v>
       </c>
@@ -3609,7 +3634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>38</v>
       </c>
@@ -3617,7 +3642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>40</v>
       </c>
@@ -3625,7 +3650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>11</v>
       </c>
@@ -3633,7 +3658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -3641,7 +3666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3649,7 +3674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15</v>
       </c>
@@ -3657,7 +3682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -3665,7 +3690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3673,7 +3698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3681,7 +3706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>39</v>
       </c>
@@ -3689,7 +3714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>18</v>
       </c>
@@ -3697,7 +3722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>11</v>
       </c>
@@ -3705,7 +3730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -3713,7 +3738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3721,7 +3746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>21</v>
       </c>
@@ -3729,7 +3754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3737,7 +3762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>39</v>
       </c>
@@ -3745,7 +3770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>28</v>
       </c>
@@ -3753,7 +3778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>32</v>
       </c>
@@ -3761,7 +3786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>16</v>
       </c>
@@ -3769,7 +3794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>30</v>
       </c>
@@ -3777,7 +3802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>13</v>
       </c>
@@ -3785,7 +3810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>21</v>
       </c>
@@ -3793,7 +3818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3801,7 +3826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>22</v>
       </c>
@@ -3809,7 +3834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>35</v>
       </c>
@@ -3817,7 +3842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3825,7 +3850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>32</v>
       </c>
@@ -3833,7 +3858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
@@ -3841,7 +3866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3849,7 +3874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>21</v>
       </c>
@@ -3857,7 +3882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>27</v>
       </c>
@@ -3865,7 +3890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>26</v>
       </c>
@@ -3873,7 +3898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>23</v>
       </c>
@@ -3881,7 +3906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3889,7 +3914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>19</v>
       </c>
@@ -3897,7 +3922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>37</v>
       </c>
@@ -3905,7 +3930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>25</v>
       </c>
@@ -3913,7 +3938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>34</v>
       </c>
@@ -3921,7 +3946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -3929,7 +3954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>19</v>
       </c>
@@ -3937,7 +3962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>8</v>
       </c>
@@ -3945,7 +3970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>27</v>
       </c>
@@ -3953,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>3</v>
       </c>
@@ -3961,7 +3986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -3969,7 +3994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>32</v>
       </c>
@@ -3977,7 +4002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5</v>
       </c>
@@ -3985,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>30</v>
       </c>
@@ -3993,7 +4018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>18</v>
       </c>
@@ -4001,7 +4026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>20</v>
       </c>
@@ -4009,7 +4034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>34</v>
       </c>
@@ -4017,7 +4042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>35</v>
       </c>
@@ -4025,7 +4050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>5</v>
       </c>
@@ -4033,7 +4058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>9</v>
       </c>
@@ -4041,7 +4066,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>19</v>
       </c>
@@ -4049,7 +4074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>27</v>
       </c>
@@ -4057,7 +4082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>22</v>
       </c>
@@ -4065,7 +4090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>35</v>
       </c>
@@ -4073,7 +4098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4081,7 +4106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>8</v>
       </c>
@@ -4089,7 +4114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>21</v>
       </c>
@@ -4097,7 +4122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>33</v>
       </c>
@@ -4105,7 +4130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>34</v>
       </c>
@@ -4113,7 +4138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>12</v>
       </c>
@@ -4121,7 +4146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>8</v>
       </c>
@@ -4129,7 +4154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>24</v>
       </c>
@@ -4137,7 +4162,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>40</v>
       </c>
@@ -4145,7 +4170,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>5</v>
       </c>
@@ -4153,7 +4178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>13</v>
       </c>
@@ -4161,7 +4186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>34</v>
       </c>
@@ -4169,7 +4194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>39</v>
       </c>
@@ -4177,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1</v>
       </c>
@@ -4185,7 +4210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>24</v>
       </c>
@@ -4193,7 +4218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>39</v>
       </c>
@@ -4201,7 +4226,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>8</v>
       </c>
@@ -4209,7 +4234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>37</v>
       </c>
@@ -4217,7 +4242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>17</v>
       </c>
@@ -4225,7 +4250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>16</v>
       </c>
@@ -4233,7 +4258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>31</v>
       </c>
@@ -4241,7 +4266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>6</v>
       </c>
@@ -4249,7 +4274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>13</v>
       </c>
@@ -4257,7 +4282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>3</v>
       </c>
@@ -4265,7 +4290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>6</v>
       </c>
@@ -4273,7 +4298,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8</v>
       </c>
@@ -4281,7 +4306,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>16</v>
       </c>
@@ -4289,7 +4314,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>13</v>
       </c>
@@ -4297,7 +4322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>37</v>
       </c>
@@ -4305,7 +4330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>33</v>
       </c>
@@ -4313,7 +4338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>18</v>
       </c>
@@ -4321,7 +4346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>37</v>
       </c>
@@ -4329,7 +4354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>23</v>
       </c>
@@ -4337,7 +4362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>33</v>
       </c>
@@ -4345,7 +4370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>10</v>
       </c>
@@ -4353,7 +4378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>7</v>
       </c>
@@ -4361,7 +4386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>17</v>
       </c>
@@ -4369,7 +4394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>16</v>
       </c>
@@ -4377,7 +4402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>16</v>
       </c>
@@ -4391,14 +4416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>156</v>
       </c>
@@ -4406,7 +4431,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>17</v>
       </c>
@@ -4414,7 +4439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
@@ -4422,7 +4447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>14</v>
       </c>
@@ -4430,7 +4455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
@@ -4438,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>17</v>
       </c>
@@ -4446,7 +4471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>18</v>
       </c>
@@ -4454,7 +4479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>14</v>
       </c>
@@ -4462,7 +4487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>22</v>
       </c>
@@ -4470,7 +4495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>25</v>
       </c>
@@ -4478,7 +4503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -4486,7 +4511,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>23</v>
       </c>
@@ -4494,7 +4519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>29</v>
       </c>
@@ -4502,7 +4527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20</v>
       </c>
@@ -4510,7 +4535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4518,7 +4543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4526,7 +4551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>25</v>
       </c>
@@ -4534,7 +4559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>23</v>
       </c>
@@ -4542,7 +4567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>13</v>
       </c>
@@ -4550,7 +4575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>8</v>
       </c>
@@ -4558,7 +4583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9</v>
       </c>
@@ -4566,7 +4591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4574,7 +4599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -4582,7 +4607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -4590,7 +4615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>28</v>
       </c>
@@ -4598,7 +4623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -4606,7 +4631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -4614,7 +4639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -4622,7 +4647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>17</v>
       </c>
@@ -4630,7 +4655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -4638,7 +4663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>27</v>
       </c>
@@ -4646,7 +4671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>14</v>
       </c>
@@ -4654,7 +4679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>28</v>
       </c>
@@ -4662,7 +4687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>30</v>
       </c>
@@ -4670,7 +4695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>9</v>
       </c>
@@ -4678,7 +4703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>22</v>
       </c>
@@ -4686,7 +4711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>15</v>
       </c>
@@ -4694,7 +4719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>30</v>
       </c>
@@ -4702,7 +4727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>25</v>
       </c>
@@ -4710,7 +4735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>19</v>
       </c>
@@ -4718,7 +4743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>17</v>
       </c>
@@ -4726,7 +4751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>21</v>
       </c>
@@ -4734,7 +4759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>16</v>
       </c>
@@ -4742,7 +4767,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>15</v>
       </c>
@@ -4750,7 +4775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>27</v>
       </c>
@@ -4758,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5</v>
       </c>
@@ -4766,7 +4791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -4774,7 +4799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>9</v>
       </c>
@@ -4782,7 +4807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>18</v>
       </c>
@@ -4790,7 +4815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>9</v>
       </c>
@@ -4798,7 +4823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>9</v>
       </c>
@@ -4806,7 +4831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>14</v>
       </c>
@@ -4814,7 +4839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>8</v>
       </c>
@@ -4822,7 +4847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>14</v>
       </c>
@@ -4830,7 +4855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>27</v>
       </c>
@@ -4838,7 +4863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>16</v>
       </c>
@@ -4846,7 +4871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>17</v>
       </c>
@@ -4854,7 +4879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>9</v>
       </c>
@@ -4862,7 +4887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>28</v>
       </c>
@@ -4870,7 +4895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>16</v>
       </c>
@@ -4878,7 +4903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2</v>
       </c>
@@ -4886,7 +4911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>12</v>
       </c>
@@ -4894,7 +4919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>27</v>
       </c>
@@ -4902,7 +4927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>8</v>
       </c>
@@ -4910,7 +4935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
@@ -4918,7 +4943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3</v>
       </c>
@@ -4926,7 +4951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>18</v>
       </c>
@@ -4934,7 +4959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>18</v>
       </c>
@@ -4942,7 +4967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>17</v>
       </c>
@@ -4950,7 +4975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>12</v>
       </c>
@@ -4958,7 +4983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>25</v>
       </c>
@@ -4966,7 +4991,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>15</v>
       </c>
@@ -4974,7 +4999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>16</v>
       </c>
@@ -4982,7 +5007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10</v>
       </c>
@@ -4990,7 +5015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>17</v>
       </c>
@@ -4998,7 +5023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>12</v>
       </c>
@@ -5006,7 +5031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>17</v>
       </c>
@@ -5014,7 +5039,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>20</v>
       </c>
@@ -5022,7 +5047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>3</v>
       </c>
@@ -5030,7 +5055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>10</v>
       </c>
@@ -5038,7 +5063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2</v>
       </c>
@@ -5046,7 +5071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>16</v>
       </c>
@@ -5054,7 +5079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>26</v>
       </c>
@@ -5062,7 +5087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
@@ -5070,7 +5095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>25</v>
       </c>
@@ -5078,7 +5103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>17</v>
       </c>
@@ -5086,7 +5111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>3</v>
       </c>
@@ -5094,7 +5119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>12</v>
       </c>
@@ -5102,7 +5127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>14</v>
       </c>
@@ -5110,7 +5135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1</v>
       </c>
@@ -5118,7 +5143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>17</v>
       </c>
@@ -5126,7 +5151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>22</v>
       </c>
@@ -5134,7 +5159,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2</v>
       </c>
@@ -5142,7 +5167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>28</v>
       </c>
@@ -5150,7 +5175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>24</v>
       </c>
@@ -5158,7 +5183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>18</v>
       </c>
@@ -5166,7 +5191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1</v>
       </c>
@@ -5174,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>24</v>
       </c>
@@ -5182,7 +5207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>17</v>
       </c>
@@ -5190,7 +5215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>19</v>
       </c>
@@ -5198,7 +5223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>22</v>
       </c>
@@ -5212,14 +5237,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>125</v>
       </c>
@@ -5227,7 +5252,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15</v>
       </c>
@@ -5235,7 +5260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>14</v>
       </c>
@@ -5243,7 +5268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>19</v>
       </c>
@@ -5251,7 +5276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -5259,7 +5284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5267,7 +5292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8</v>
       </c>
@@ -5275,7 +5300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>14</v>
       </c>
@@ -5283,7 +5308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -5291,7 +5316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -5299,7 +5324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -5307,7 +5332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>17</v>
       </c>
@@ -5315,7 +5340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5323,7 +5348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -5331,7 +5356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -5339,7 +5364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -5347,7 +5372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5355,7 +5380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -5363,7 +5388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -5371,7 +5396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6</v>
       </c>
@@ -5379,7 +5404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5387,7 +5412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10</v>
       </c>
@@ -5395,7 +5420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5403,7 +5428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10</v>
       </c>
@@ -5411,7 +5436,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>16</v>
       </c>
@@ -5419,7 +5444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>16</v>
       </c>
@@ -5427,7 +5452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -5435,7 +5460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>12</v>
       </c>
@@ -5443,7 +5468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -5451,7 +5476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>12</v>
       </c>
@@ -5459,7 +5484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -5467,7 +5492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -5475,7 +5500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>11</v>
       </c>
@@ -5483,7 +5508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>14</v>
       </c>
@@ -5491,7 +5516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10</v>
       </c>
@@ -5499,7 +5524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>6</v>
       </c>
@@ -5507,7 +5532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>18</v>
       </c>
@@ -5515,7 +5540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>14</v>
       </c>
@@ -5523,7 +5548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7</v>
       </c>
@@ -5531,7 +5556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>19</v>
       </c>
@@ -5539,7 +5564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3</v>
       </c>
@@ -5547,7 +5572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>12</v>
       </c>
@@ -5555,7 +5580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>8</v>
       </c>
@@ -5563,7 +5588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>11</v>
       </c>
@@ -5571,7 +5596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>19</v>
       </c>
@@ -5579,7 +5604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>17</v>
       </c>
@@ -5587,7 +5612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>15</v>
       </c>
@@ -5595,7 +5620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>15</v>
       </c>
@@ -5603,7 +5628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4</v>
       </c>
@@ -5611,7 +5636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>7</v>
       </c>
@@ -5619,7 +5644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>9</v>
       </c>
@@ -5627,7 +5652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>18</v>
       </c>
@@ -5635,7 +5660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>16</v>
       </c>
@@ -5643,7 +5668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>7</v>
       </c>
@@ -5651,7 +5676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>13</v>
       </c>
@@ -5659,7 +5684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>5</v>
       </c>
@@ -5667,7 +5692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>17</v>
       </c>
@@ -5675,7 +5700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5</v>
       </c>
@@ -5683,7 +5708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10</v>
       </c>
@@ -5691,7 +5716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>8</v>
       </c>
@@ -5699,7 +5724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
@@ -5707,7 +5732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>16</v>
       </c>
@@ -5715,7 +5740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>12</v>
       </c>
@@ -5723,7 +5748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>19</v>
       </c>
@@ -5731,7 +5756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>15</v>
       </c>
@@ -5739,7 +5764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6</v>
       </c>
@@ -5747,7 +5772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>19</v>
       </c>
@@ -5755,7 +5780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>18</v>
       </c>
@@ -5763,7 +5788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1</v>
       </c>
@@ -5771,7 +5796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20</v>
       </c>
@@ -5779,7 +5804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2</v>
       </c>
@@ -5787,7 +5812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>12</v>
       </c>
@@ -5795,7 +5820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10</v>
       </c>
@@ -5803,7 +5828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>15</v>
       </c>
@@ -5811,7 +5836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>13</v>
       </c>
@@ -5819,7 +5844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3</v>
       </c>
@@ -5827,7 +5852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>12</v>
       </c>
@@ -5835,7 +5860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1</v>
       </c>
@@ -5843,7 +5868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>5</v>
       </c>
@@ -5851,7 +5876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2</v>
       </c>
@@ -5859,7 +5884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>18</v>
       </c>
@@ -5867,7 +5892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>19</v>
       </c>
@@ -5875,7 +5900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>19</v>
       </c>
@@ -5883,7 +5908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>11</v>
       </c>
@@ -5891,7 +5916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>14</v>
       </c>
@@ -5899,7 +5924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>10</v>
       </c>
@@ -5907,7 +5932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>14</v>
       </c>
@@ -5915,7 +5940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>17</v>
       </c>
@@ -5923,7 +5948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>7</v>
       </c>
@@ -5931,7 +5956,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1</v>
       </c>
@@ -5939,7 +5964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>10</v>
       </c>
@@ -5947,7 +5972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>14</v>
       </c>
@@ -5955,7 +5980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>5</v>
       </c>
@@ -5963,7 +5988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>5</v>
       </c>
@@ -5971,7 +5996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>11</v>
       </c>
@@ -5979,7 +6004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>15</v>
       </c>
@@ -5987,7 +6012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>5</v>
       </c>
@@ -5995,7 +6020,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>18</v>
       </c>
@@ -6003,7 +6028,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4</v>
       </c>
@@ -6011,7 +6036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>7</v>
       </c>
@@ -6019,7 +6044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>9</v>
       </c>
@@ -6033,14 +6058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>273</v>
       </c>
@@ -6048,7 +6073,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6056,7 +6081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -6064,7 +6089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6072,7 +6097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6080,7 +6105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -6088,7 +6113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -6096,7 +6121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -6104,7 +6129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -6112,7 +6137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -6120,7 +6145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6128,7 +6153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -6136,7 +6161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
@@ -6144,7 +6169,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -6152,7 +6177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -6160,7 +6185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
@@ -6168,7 +6193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -6176,7 +6201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
@@ -6184,7 +6209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -6192,7 +6217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -6200,7 +6225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -6208,7 +6233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10</v>
       </c>
@@ -6216,7 +6241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -6224,7 +6249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -6232,7 +6257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -6240,7 +6265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -6248,7 +6273,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -6256,7 +6281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8</v>
       </c>
@@ -6264,7 +6289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -6272,7 +6297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
@@ -6280,7 +6305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10</v>
       </c>
@@ -6288,7 +6313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -6296,7 +6321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -6304,7 +6329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -6312,7 +6337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -6320,7 +6345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
@@ -6328,7 +6353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>6</v>
       </c>
@@ -6336,7 +6361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -6344,7 +6369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>9</v>
       </c>
@@ -6352,7 +6377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>7</v>
       </c>
@@ -6360,7 +6385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -6368,7 +6393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -6376,7 +6401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4</v>
       </c>
@@ -6384,7 +6409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>6</v>
       </c>
@@ -6392,7 +6417,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -6400,7 +6425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>4</v>
       </c>
@@ -6408,7 +6433,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -6416,7 +6441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>6</v>
       </c>
@@ -6424,7 +6449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -6432,7 +6457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>6</v>
       </c>
@@ -6440,7 +6465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1</v>
       </c>
@@ -6448,7 +6473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -6456,7 +6481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>7</v>
       </c>
@@ -6464,7 +6489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>8</v>
       </c>
@@ -6472,7 +6497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>3</v>
       </c>
@@ -6480,7 +6505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>7</v>
       </c>
@@ -6488,7 +6513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1</v>
       </c>
@@ -6496,7 +6521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>7</v>
       </c>
@@ -6504,7 +6529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
@@ -6512,7 +6537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>4</v>
       </c>
@@ -6520,7 +6545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>10</v>
       </c>
@@ -6528,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>7</v>
       </c>
@@ -6536,7 +6561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3</v>
       </c>
@@ -6544,7 +6569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6</v>
       </c>
@@ -6552,7 +6577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
@@ -6560,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>4</v>
       </c>
@@ -6568,7 +6593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>8</v>
       </c>
@@ -6576,7 +6601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4</v>
       </c>
@@ -6584,7 +6609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1</v>
       </c>
@@ -6592,7 +6617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1</v>
       </c>
@@ -6600,7 +6625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2</v>
       </c>
@@ -6608,7 +6633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>6</v>
       </c>
@@ -6616,7 +6641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3</v>
       </c>
@@ -6624,7 +6649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1</v>
       </c>
@@ -6632,7 +6657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -6640,7 +6665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>6</v>
       </c>
@@ -6648,7 +6673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>5</v>
       </c>
@@ -6656,7 +6681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>3</v>
       </c>
@@ -6664,7 +6689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1</v>
       </c>
@@ -6672,7 +6697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1</v>
       </c>
@@ -6680,7 +6705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>6</v>
       </c>
@@ -6688,7 +6713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>8</v>
       </c>
@@ -6696,7 +6721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>5</v>
       </c>
@@ -6704,7 +6729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>10</v>
       </c>
@@ -6712,7 +6737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>10</v>
       </c>
@@ -6720,7 +6745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>9</v>
       </c>
@@ -6728,7 +6753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>10</v>
       </c>
@@ -6736,7 +6761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>5</v>
       </c>
@@ -6744,7 +6769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>6</v>
       </c>
@@ -6752,7 +6777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>7</v>
       </c>
@@ -6760,7 +6785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -6768,7 +6793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2</v>
       </c>
@@ -6776,7 +6801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
@@ -6784,7 +6809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>7</v>
       </c>
@@ -6792,7 +6817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>9</v>
       </c>
@@ -6800,7 +6825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>5</v>
       </c>
@@ -6808,7 +6833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>3</v>
       </c>
@@ -6816,7 +6841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>6</v>
       </c>
@@ -6824,7 +6849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>5</v>
       </c>
@@ -6832,7 +6857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>5</v>
       </c>
@@ -6840,7 +6865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1</v>
       </c>

</xml_diff>